<commit_message>
add autoscaling first decision
</commit_message>
<xml_diff>
--- a/data-set/i-0cc45b1c3d48b7828.xlsx
+++ b/data-set/i-0cc45b1c3d48b7828.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -831,6 +831,2414 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>20:39:07</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2.1667</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>20:39:27</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2.1667</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>20:47:13</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2.1667</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3326.0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3052.0</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>20:48:01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3506.0</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3104.0</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>20:49:10</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2.1667</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>6188.0</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>5846.0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>20:50:10</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>3740.0</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3209.0</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>20:51:11</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3740.0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>3209.0</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>20:52:11</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2.2034</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3450.0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>3076.0</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>20:53:10</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>20:54:10</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>5014.0</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>4313.0</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>20:55:10</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2.1667</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>3482.0</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>3128.0</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>20:56:10</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2.2951</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>3754.0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2837.0</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>20:57:10</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1.8644</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>3754.0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2837.0</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>20:58:10</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>4752.0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>4612.0</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>20:59:10</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2.459</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>8597.0</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>8955.0</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>20:59:50</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2.459</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>21:00:37</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1.8644</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>21:06:17</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2.3333</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>21:10:01</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2.1667</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>21:25:00</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2.2034</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>3392.0</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>3052.0</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>21:26:09</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>3416.0</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>3128.0</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>21:26:40</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>3416.0</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>3128.0</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>21:27:49</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>3494.0</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>3136.0</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>21:28:48</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>3494.0</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>3136.0</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>21:29:49</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>3640.0</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>3140.0</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>21:30:48</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>3450.0</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>3076.0</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>21:31:48</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2.3729</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>3450.0</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>3076.0</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>21:32:48</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3270.0</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>3024.0</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>02:21:39</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>5945.0</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>6118.0</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>02:22:18</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>5591.0</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>5942.0</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>02:22:39</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>5591.0</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>5942.0</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>02:24:18</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>2.2951</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>5681.0</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>6018.0</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>02:25:19</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>2.2034</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>02:27:00</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>3492.0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>02:27:00</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>3492.0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>02:28:22</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>02:28:23</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>02:28:23</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>02:28:24</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>02:28:25</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>02:28:52</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>02:28:53</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>3304.0</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>02:29:05</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>02:29:06</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>02:29:21</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>02:29:22</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>02:29:32</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>02:29:32</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>02:29:33</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>02:30:18</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>2</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>02:30:19</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>2</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>02:30:20</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>2</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>02:30:20</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>2</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>02:30:21</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>2</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>02:31:27</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>2</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>02:31:28</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>2</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>02:31:28</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>2</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>02:31:29</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>2</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>02:32:49</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>02:32:49</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>02:32:50</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>02:32:51</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>02:32:51</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>3360.0</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>02:34:32</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>02:34:32</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>02:34:33</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>02:34:34</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>02:34:43</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>3000.0</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>02:35:44</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>3064.0</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2860.0</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>02:40:20</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>3438.0</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>3008.0</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>02:41:21</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>3528.0</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>3184.0</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>02:53:50</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>3594.0</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>3184.0</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>02:58:22</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>5868.0</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>6145.0</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>02:59:20</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>3370.0</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>02:59:41</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>3370.0</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2972.0</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>03:00:52</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>2.3333</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>4558.0</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>3874.0</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>03:01:13</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>03:01:33</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>03:01:54</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>2.459</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>3426.0</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>3100.0</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add checks for trigger escalability
</commit_message>
<xml_diff>
--- a/data-set/i-0cc45b1c3d48b7828.xlsx
+++ b/data-set/i-0cc45b1c3d48b7828.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3239,6 +3239,246 @@
         </is>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>03:08:44</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>3572.0</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>03:10:38</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>3416.0</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>3028.0</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>03:11:15</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>2.1311</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>3416.0</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>3028.0</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>03:12:53</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>2.3729</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>3638.0</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>3204.0</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>03:13:18</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>7042.0</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>6843.0</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>03:13:39</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>7042.0</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>6843.0</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>03:14:00</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>7042.0</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>6843.0</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2021-04-06</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>03:14:21</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>2.1667</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>7042.0</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>6843.0</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>InService</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>